<commit_message>
docs: Updated data dict
</commit_message>
<xml_diff>
--- a/src/db/data_dict_batiment.xlsx
+++ b/src/db/data_dict_batiment.xlsx
@@ -1376,7 +1376,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1569,7 +1569,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>code_dpt</t>
+          <t>code_epci</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1582,19 +1582,19 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Code département</t>
+          <t>Identifiant EPCI (établissements publics de coopération intercommunale) INSEE</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>statut</t>
+          <t>code_dpt</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>rnb.statut_batiment</t>
+          <t>TEXT</t>
         </is>
       </c>
       <c r="C11" t="b">
@@ -1602,19 +1602,19 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Statut du batiment relativement à la liste des champs possible</t>
+          <t>Code département</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>localisation</t>
+          <t>statut</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>geometry(POINT,2154)</t>
+          <t>rnb.statut_batiment</t>
         </is>
       </c>
       <c r="C12" t="b">
@@ -1622,30 +1622,34 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Localisant du batiment. Par défaut, il s agit du point à l inteieur du batiment, le plus proche du centroide de la géométrie du batiment</t>
+          <t>Statut du batiment relativement à la liste des champs possible</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>dt_deb</t>
+          <t>localisation</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>DATE</t>
+          <t>geometry(POINT,2154)</t>
         </is>
       </c>
       <c r="C13" t="b">
         <v>1</v>
       </c>
-      <c r="D13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Localisant du batiment. Par défaut, il s agit du point à l inteieur du batiment, le plus proche du centroide de la géométrie du batiment</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>dt_fin</t>
+          <t>dt_deb</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1661,27 +1665,23 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>id_tup</t>
+          <t>dt_fin</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>TEXT</t>
+          <t>DATE</t>
         </is>
       </c>
       <c r="C15" t="b">
         <v>1</v>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>clef étrangère de la table des TUPs</t>
-        </is>
-      </c>
+      <c r="D15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>id_bdnb</t>
+          <t>id_tup</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1694,25 +1694,45 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>clef étrangère de l id batiment bdnb du CSTB</t>
+          <t>clef étrangère de la table des TUPs</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>id_bdnb</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>TEXT</t>
+        </is>
+      </c>
+      <c r="C17" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>clef étrangère de l id batiment bdnb du CSTB</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
           <t>geombat</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B18" t="inlineStr">
         <is>
           <t>geometry(MULTIPOLYGON,2154)</t>
         </is>
       </c>
-      <c r="C17" t="b">
-        <v>1</v>
-      </c>
-      <c r="D17" t="inlineStr">
+      <c r="C18" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" t="inlineStr">
         <is>
           <t>Géometrie du batiment</t>
         </is>

</xml_diff>